<commit_message>
Update scale UI for visiblity on laptop screen and adjusted days to look back
</commit_message>
<xml_diff>
--- a/QualityImprovementMonitor/QualityMetricsHistory.xlsx
+++ b/QualityImprovementMonitor/QualityMetricsHistory.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>04-Jan-2019</t>
+  </si>
+  <si>
+    <t>05-Jan-2019</t>
   </si>
   <si>
     <t>23-Oct-2018</t>
@@ -525,7 +528,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -712,6 +715,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -723,7 +770,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -910,6 +957,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -921,7 +1012,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1108,6 +1199,50 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1119,7 +1254,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1306,6 +1441,50 @@
         <v>6600</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>3336</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>420</v>
+      </c>
+      <c r="E5" t="n">
+        <v>313</v>
+      </c>
+      <c r="F5" t="n">
+        <v>378</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>133</v>
+      </c>
+      <c r="I5" t="n">
+        <v>24</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1390</v>
+      </c>
+      <c r="K5" t="n">
+        <v>24</v>
+      </c>
+      <c r="L5" t="n">
+        <v>549</v>
+      </c>
+      <c r="M5" t="n">
+        <v>33</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -1317,7 +1496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:N60"/>
@@ -2647,7 +2826,7 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B31" t="n">
         <v>10</v>
@@ -2691,7 +2870,7 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B32" t="n">
         <v>10</v>
@@ -2735,7 +2914,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B33" t="n">
         <v>10</v>
@@ -2779,7 +2958,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" t="n">
         <v>10</v>
@@ -2823,7 +3002,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B35" t="n">
         <v>10</v>
@@ -2867,7 +3046,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B36" t="n">
         <v>10</v>
@@ -2911,7 +3090,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B37" t="n">
         <v>10</v>
@@ -2999,7 +3178,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B39" t="n">
         <v>10</v>
@@ -3043,7 +3222,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B40" t="n">
         <v>10</v>
@@ -3087,7 +3266,7 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B41" t="n">
         <v>10</v>
@@ -3131,7 +3310,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B42" t="n">
         <v>10</v>
@@ -3175,7 +3354,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B43" t="n">
         <v>10</v>
@@ -3219,7 +3398,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B44" t="n">
         <v>10</v>
@@ -3263,7 +3442,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B45" t="n">
         <v>10</v>
@@ -3307,7 +3486,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B46" t="n">
         <v>10</v>
@@ -3351,7 +3530,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B47" t="n">
         <v>10</v>
@@ -3395,7 +3574,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B48" t="n">
         <v>10</v>
@@ -3439,7 +3618,7 @@
     </row>
     <row r="49" spans="1:14">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B49" t="n">
         <v>10</v>
@@ -3483,7 +3662,7 @@
     </row>
     <row r="50" spans="1:14">
       <c r="A50" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B50" t="n">
         <v>10</v>
@@ -3527,7 +3706,7 @@
     </row>
     <row r="51" spans="1:14">
       <c r="A51" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B51" t="n">
         <v>10</v>
@@ -3571,7 +3750,7 @@
     </row>
     <row r="52" spans="1:14">
       <c r="A52" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B52" t="n">
         <v>10</v>
@@ -3615,7 +3794,7 @@
     </row>
     <row r="53" spans="1:14">
       <c r="A53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B53" t="n">
         <v>10</v>
@@ -3659,7 +3838,7 @@
     </row>
     <row r="54" spans="1:14">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B54" t="n">
         <v>10</v>
@@ -3703,7 +3882,7 @@
     </row>
     <row r="55" spans="1:14">
       <c r="A55" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B55" t="n">
         <v>10</v>
@@ -3747,7 +3926,7 @@
     </row>
     <row r="56" spans="1:14">
       <c r="A56" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B56" t="n">
         <v>10</v>
@@ -3791,7 +3970,7 @@
     </row>
     <row r="57" spans="1:14">
       <c r="A57" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B57" t="n">
         <v>10</v>
@@ -3835,7 +4014,7 @@
     </row>
     <row r="58" spans="1:14">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B58" t="n">
         <v>9</v>
@@ -3879,7 +4058,7 @@
     </row>
     <row r="59" spans="1:14">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B59" t="n">
         <v>9</v>
@@ -3923,7 +4102,7 @@
     </row>
     <row r="60" spans="1:14">
       <c r="A60" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B60" t="n">
         <v>9</v>
@@ -4051,6 +4230,50 @@
       </c>
       <c r="N62" t="n">
         <v>190</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14">
+      <c r="A63" t="s">
+        <v>16</v>
+      </c>
+      <c r="B63" t="n">
+        <v>9</v>
+      </c>
+      <c r="C63" t="n">
+        <v>0</v>
+      </c>
+      <c r="D63" t="n">
+        <v>8</v>
+      </c>
+      <c r="E63" t="n">
+        <v>16</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0</v>
+      </c>
+      <c r="G63" t="n">
+        <v>9</v>
+      </c>
+      <c r="H63" t="n">
+        <v>17</v>
+      </c>
+      <c r="I63" t="n">
+        <v>2</v>
+      </c>
+      <c r="J63" t="n">
+        <v>51</v>
+      </c>
+      <c r="K63" t="n">
+        <v>30</v>
+      </c>
+      <c r="L63" t="n">
+        <v>12</v>
+      </c>
+      <c r="M63" t="n">
+        <v>33</v>
+      </c>
+      <c r="N63" t="n">
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4064,7 +4287,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:N22"/>
@@ -4118,7 +4341,7 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" t="n">
         <v>458</v>
@@ -4162,7 +4385,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="n">
         <v>458</v>
@@ -4206,7 +4429,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="n">
         <v>458</v>
@@ -4250,7 +4473,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" t="n">
         <v>458</v>
@@ -4294,7 +4517,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" t="n">
         <v>458</v>
@@ -4338,7 +4561,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" t="n">
         <v>461</v>
@@ -4382,7 +4605,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="n">
         <v>461</v>
@@ -4426,7 +4649,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B9" t="n">
         <v>461</v>
@@ -4470,7 +4693,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" t="n">
         <v>461</v>
@@ -4514,7 +4737,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B11" t="n">
         <v>461</v>
@@ -4558,7 +4781,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B12" t="n">
         <v>461</v>
@@ -4602,7 +4825,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" t="n">
         <v>461</v>
@@ -4646,7 +4869,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B14" t="n">
         <v>461</v>
@@ -4690,7 +4913,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B15" t="n">
         <v>461</v>
@@ -4734,7 +4957,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B16" t="n">
         <v>461</v>
@@ -4778,7 +5001,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B17" t="n">
         <v>461</v>
@@ -4822,7 +5045,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B18" t="n">
         <v>461</v>
@@ -4866,7 +5089,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" t="n">
         <v>461</v>
@@ -4910,7 +5133,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" t="n">
         <v>461</v>
@@ -4954,7 +5177,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B21" t="n">
         <v>461</v>
@@ -4998,7 +5221,7 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B22" t="n">
         <v>461</v>
@@ -5126,6 +5349,50 @@
       </c>
       <c r="N24" t="n">
         <v>2098</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" t="n">
+        <v>461</v>
+      </c>
+      <c r="C25" t="n">
+        <v>54</v>
+      </c>
+      <c r="D25" t="n">
+        <v>127</v>
+      </c>
+      <c r="E25" t="n">
+        <v>66</v>
+      </c>
+      <c r="F25" t="n">
+        <v>62</v>
+      </c>
+      <c r="G25" t="n">
+        <v>23</v>
+      </c>
+      <c r="H25" t="n">
+        <v>290</v>
+      </c>
+      <c r="I25" t="n">
+        <v>17</v>
+      </c>
+      <c r="J25" t="n">
+        <v>282</v>
+      </c>
+      <c r="K25" t="n">
+        <v>163</v>
+      </c>
+      <c r="L25" t="n">
+        <v>537</v>
+      </c>
+      <c r="M25" t="n">
+        <v>14</v>
+      </c>
+      <c r="N25" t="n">
+        <v>2096</v>
       </c>
     </row>
   </sheetData>
@@ -5139,7 +5406,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5326,6 +5593,50 @@
         <v>1021</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>6</v>
+      </c>
+      <c r="F5" t="n">
+        <v>23</v>
+      </c>
+      <c r="G5" t="n">
+        <v>92</v>
+      </c>
+      <c r="H5" t="n">
+        <v>277</v>
+      </c>
+      <c r="I5" t="n">
+        <v>16</v>
+      </c>
+      <c r="J5" t="n">
+        <v>83</v>
+      </c>
+      <c r="K5" t="n">
+        <v>214</v>
+      </c>
+      <c r="L5" t="n">
+        <v>297</v>
+      </c>
+      <c r="M5" t="n">
+        <v>4</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1021</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
@@ -5337,7 +5648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -5524,6 +5835,50 @@
         <v>518</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>38</v>
+      </c>
+      <c r="C5" t="n">
+        <v>156</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>319</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>2</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>518</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove invalid line from Quality metrics history excel sheet
</commit_message>
<xml_diff>
--- a/QualityImprovementMonitor/QualityMetricsHistory.xlsx
+++ b/QualityImprovementMonitor/QualityMetricsHistory.xlsx
@@ -272,9 +272,6 @@
     <t>03-May-2019</t>
   </si>
   <si>
-    <t>06-May-2019</t>
-  </si>
-  <si>
     <t>07-May-2019</t>
   </si>
   <si>
@@ -363,6 +360,9 @@
   </si>
   <si>
     <t>24-Dec-2018</t>
+  </si>
+  <si>
+    <t>06-May-2019</t>
   </si>
 </sst>
 </file>
@@ -732,10 +732,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D48"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -4041,10 +4041,10 @@
         <v>83</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
@@ -4053,7 +4053,7 @@
         <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G71" t="n">
         <v>0</v>
@@ -4062,71 +4062,24 @@
         <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="J71" t="n">
         <v>0</v>
       </c>
       <c r="K71" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L71" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="M71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="O71" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" t="n">
-        <v>15</v>
-      </c>
-      <c r="C72" t="n">
-        <v>79</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0</v>
-      </c>
-      <c r="E72" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" t="n">
-        <v>28</v>
-      </c>
-      <c r="G72" t="n">
-        <v>0</v>
-      </c>
-      <c r="H72" t="n">
-        <v>0</v>
-      </c>
-      <c r="I72" t="n">
-        <v>116</v>
-      </c>
-      <c r="J72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K72" t="n">
-        <v>7</v>
-      </c>
-      <c r="L72" t="n">
-        <v>11</v>
-      </c>
-      <c r="M72" t="n">
-        <v>1</v>
-      </c>
-      <c r="N72" t="n">
-        <v>2</v>
-      </c>
-      <c r="O72" t="n">
         <v>259</v>
       </c>
     </row>
@@ -4141,10 +4094,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D48"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -7450,92 +7403,45 @@
         <v>83</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H71" t="n">
         <v>0</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K71" t="n">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="L71" t="n">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="M71" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O71" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" t="n">
-        <v>145</v>
-      </c>
-      <c r="C72" t="n">
-        <v>87</v>
-      </c>
-      <c r="D72" t="n">
-        <v>3</v>
-      </c>
-      <c r="E72" t="n">
-        <v>21</v>
-      </c>
-      <c r="F72" t="n">
-        <v>96</v>
-      </c>
-      <c r="G72" t="n">
-        <v>33</v>
-      </c>
-      <c r="H72" t="n">
-        <v>0</v>
-      </c>
-      <c r="I72" t="n">
-        <v>131</v>
-      </c>
-      <c r="J72" t="n">
-        <v>6</v>
-      </c>
-      <c r="K72" t="n">
-        <v>147</v>
-      </c>
-      <c r="L72" t="n">
-        <v>36</v>
-      </c>
-      <c r="M72" t="n">
-        <v>37</v>
-      </c>
-      <c r="N72" t="n">
-        <v>13</v>
-      </c>
-      <c r="O72" t="n">
         <v>755</v>
       </c>
     </row>
@@ -7550,10 +7456,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D48"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -10859,92 +10765,45 @@
         <v>83</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>109</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>320</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K71" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="L71" t="n">
-        <v>0</v>
+        <v>102</v>
       </c>
       <c r="M71" t="n">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="O71" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" t="n">
-        <v>22</v>
-      </c>
-      <c r="C72" t="n">
-        <v>109</v>
-      </c>
-      <c r="D72" t="n">
-        <v>0</v>
-      </c>
-      <c r="E72" t="n">
-        <v>24</v>
-      </c>
-      <c r="F72" t="n">
-        <v>69</v>
-      </c>
-      <c r="G72" t="n">
-        <v>2</v>
-      </c>
-      <c r="H72" t="n">
-        <v>7</v>
-      </c>
-      <c r="I72" t="n">
-        <v>320</v>
-      </c>
-      <c r="J72" t="n">
-        <v>1</v>
-      </c>
-      <c r="K72" t="n">
-        <v>16</v>
-      </c>
-      <c r="L72" t="n">
-        <v>102</v>
-      </c>
-      <c r="M72" t="n">
-        <v>43</v>
-      </c>
-      <c r="N72" t="n">
-        <v>13</v>
-      </c>
-      <c r="O72" t="n">
         <v>728</v>
       </c>
     </row>
@@ -10959,10 +10818,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D48"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:XFD71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
@@ -14268,93 +14127,46 @@
         <v>83</v>
       </c>
       <c r="B71" t="n">
-        <v>0</v>
+        <v>3521</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>562</v>
       </c>
       <c r="F71" t="n">
-        <v>0</v>
+        <v>309</v>
       </c>
       <c r="G71" t="n">
-        <v>0</v>
+        <v>378</v>
       </c>
       <c r="H71" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I71" t="n">
-        <v>0</v>
+        <v>133</v>
       </c>
       <c r="J71" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K71" t="n">
-        <v>0</v>
+        <v>1384</v>
       </c>
       <c r="L71" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="M71" t="n">
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="N71" t="n">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="O71" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:16">
-      <c r="A72" t="s">
-        <v>84</v>
-      </c>
-      <c r="B72" t="n">
-        <v>3521</v>
-      </c>
-      <c r="C72" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" t="n">
-        <v>2</v>
-      </c>
-      <c r="E72" t="n">
-        <v>562</v>
-      </c>
-      <c r="F72" t="n">
-        <v>309</v>
-      </c>
-      <c r="G72" t="n">
-        <v>378</v>
-      </c>
-      <c r="H72" t="n">
-        <v>5</v>
-      </c>
-      <c r="I72" t="n">
-        <v>133</v>
-      </c>
-      <c r="J72" t="n">
-        <v>8</v>
-      </c>
-      <c r="K72" t="n">
-        <v>1384</v>
-      </c>
-      <c r="L72" t="n">
-        <v>24</v>
-      </c>
-      <c r="M72" t="n">
-        <v>323</v>
-      </c>
-      <c r="N72" t="n">
-        <v>31</v>
-      </c>
-      <c r="O72" t="n">
-        <v>6680</v>
+        <v>6679</v>
       </c>
     </row>
   </sheetData>
@@ -14370,7 +14182,7 @@
   </sheetPr>
   <dimension ref="A1:P130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D106"/>
     </sheetView>
   </sheetViews>
@@ -15788,7 +15600,7 @@
     </row>
     <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" t="n">
         <v>10</v>
@@ -15835,7 +15647,7 @@
     </row>
     <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B32" t="n">
         <v>10</v>
@@ -15882,7 +15694,7 @@
     </row>
     <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" t="n">
         <v>10</v>
@@ -15929,7 +15741,7 @@
     </row>
     <row r="34" spans="1:16">
       <c r="A34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B34" t="n">
         <v>10</v>
@@ -15976,7 +15788,7 @@
     </row>
     <row r="35" spans="1:16">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B35" t="n">
         <v>10</v>
@@ -16023,7 +15835,7 @@
     </row>
     <row r="36" spans="1:16">
       <c r="A36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B36" t="n">
         <v>10</v>
@@ -16070,7 +15882,7 @@
     </row>
     <row r="37" spans="1:16">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" t="n">
         <v>10</v>
@@ -16164,7 +15976,7 @@
     </row>
     <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B39" t="n">
         <v>10</v>
@@ -16211,7 +16023,7 @@
     </row>
     <row r="40" spans="1:16">
       <c r="A40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B40" t="n">
         <v>10</v>
@@ -16258,7 +16070,7 @@
     </row>
     <row r="41" spans="1:16">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B41" t="n">
         <v>10</v>
@@ -16305,7 +16117,7 @@
     </row>
     <row r="42" spans="1:16">
       <c r="A42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B42" t="n">
         <v>10</v>
@@ -16352,7 +16164,7 @@
     </row>
     <row r="43" spans="1:16">
       <c r="A43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B43" t="n">
         <v>10</v>
@@ -16399,7 +16211,7 @@
     </row>
     <row r="44" spans="1:16">
       <c r="A44" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B44" t="n">
         <v>10</v>
@@ -16446,7 +16258,7 @@
     </row>
     <row r="45" spans="1:16">
       <c r="A45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" t="n">
         <v>10</v>
@@ -16493,7 +16305,7 @@
     </row>
     <row r="46" spans="1:16">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B46" t="n">
         <v>10</v>
@@ -16540,7 +16352,7 @@
     </row>
     <row r="47" spans="1:16">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B47" t="n">
         <v>10</v>
@@ -16587,7 +16399,7 @@
     </row>
     <row r="48" spans="1:16">
       <c r="A48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B48" t="n">
         <v>10</v>
@@ -16634,7 +16446,7 @@
     </row>
     <row r="49" spans="1:16">
       <c r="A49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B49" t="n">
         <v>10</v>
@@ -16681,7 +16493,7 @@
     </row>
     <row r="50" spans="1:16">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B50" t="n">
         <v>10</v>
@@ -16728,7 +16540,7 @@
     </row>
     <row r="51" spans="1:16">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B51" t="n">
         <v>10</v>
@@ -16775,7 +16587,7 @@
     </row>
     <row r="52" spans="1:16">
       <c r="A52" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B52" t="n">
         <v>10</v>
@@ -16822,7 +16634,7 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B53" t="n">
         <v>10</v>
@@ -16869,7 +16681,7 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B54" t="n">
         <v>10</v>
@@ -16916,7 +16728,7 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B55" t="n">
         <v>10</v>
@@ -16963,7 +16775,7 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B56" t="n">
         <v>10</v>
@@ -17010,7 +16822,7 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B57" t="n">
         <v>10</v>
@@ -17057,7 +16869,7 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B58" t="n">
         <v>9</v>
@@ -17104,7 +16916,7 @@
     </row>
     <row r="59" spans="1:16">
       <c r="A59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B59" t="n">
         <v>9</v>
@@ -17151,7 +16963,7 @@
     </row>
     <row r="60" spans="1:16">
       <c r="A60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B60" t="n">
         <v>9</v>
@@ -20397,7 +20209,7 @@
     </row>
     <row r="129" spans="1:16">
       <c r="A129" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B129" t="n">
         <v>0</v>
@@ -20444,7 +20256,7 @@
     </row>
     <row r="130" spans="1:16">
       <c r="A130" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B130" t="n">
         <v>0</v>
@@ -20502,7 +20314,7 @@
   </sheetPr>
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D68"/>
     </sheetView>
   </sheetViews>
@@ -20557,7 +20369,7 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B2" t="n">
         <v>458</v>
@@ -20604,7 +20416,7 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B3" t="n">
         <v>458</v>
@@ -20651,7 +20463,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" t="n">
         <v>458</v>
@@ -20698,7 +20510,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" t="n">
         <v>458</v>
@@ -20745,7 +20557,7 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" t="n">
         <v>458</v>
@@ -20792,7 +20604,7 @@
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" t="n">
         <v>461</v>
@@ -20839,7 +20651,7 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="n">
         <v>461</v>
@@ -20886,7 +20698,7 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="n">
         <v>461</v>
@@ -20933,7 +20745,7 @@
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B10" t="n">
         <v>461</v>
@@ -20980,7 +20792,7 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B11" t="n">
         <v>461</v>
@@ -21027,7 +20839,7 @@
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" t="n">
         <v>461</v>
@@ -21074,7 +20886,7 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" t="n">
         <v>461</v>
@@ -21121,7 +20933,7 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B14" t="n">
         <v>461</v>
@@ -21168,7 +20980,7 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B15" t="n">
         <v>461</v>
@@ -21215,7 +21027,7 @@
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B16" t="n">
         <v>461</v>
@@ -21262,7 +21074,7 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B17" t="n">
         <v>461</v>
@@ -21309,7 +21121,7 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B18" t="n">
         <v>461</v>
@@ -21356,7 +21168,7 @@
     </row>
     <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B19" t="n">
         <v>461</v>
@@ -21403,7 +21215,7 @@
     </row>
     <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B20" t="n">
         <v>461</v>
@@ -21450,7 +21262,7 @@
     </row>
     <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" t="n">
         <v>461</v>
@@ -21497,7 +21309,7 @@
     </row>
     <row r="22" spans="1:16">
       <c r="A22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B22" t="n">
         <v>461</v>
@@ -24743,7 +24555,7 @@
     </row>
     <row r="91" spans="1:16">
       <c r="A91" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B91" t="n">
         <v>489</v>
@@ -24790,7 +24602,7 @@
     </row>
     <row r="92" spans="1:16">
       <c r="A92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B92" t="n">
         <v>489</v>
@@ -24848,7 +24660,7 @@
   </sheetPr>
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D48"/>
     </sheetView>
   </sheetViews>
@@ -28152,7 +27964,7 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B71" t="n">
         <v>331</v>
@@ -28199,7 +28011,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" t="n">
         <v>331</v>
@@ -28257,7 +28069,7 @@
   </sheetPr>
   <dimension ref="A1:P72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D48"/>
     </sheetView>
   </sheetViews>
@@ -31561,7 +31373,7 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>113</v>
       </c>
       <c r="B71" t="n">
         <v>40</v>
@@ -31608,7 +31420,7 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" t="n">
         <v>40</v>

</xml_diff>